<commit_message>
More benchmarks and more about results in report
</commit_message>
<xml_diff>
--- a/Project2/report/proj2_data.xlsx
+++ b/Project2/report/proj2_data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MSU Phy Courses\Computational Physics\CompPhy_Project\Project2\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DAE3EC-D7C0-4401-8985-89AEF93740C9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900" activeTab="1" xr2:uid="{25EEB7D5-7CE5-46B3-8B31-600E895F7528}"/>
   </bookViews>
   <sheets>
     <sheet name="one" sheetId="2" r:id="rId1"/>
-    <sheet name="two" sheetId="3" r:id="rId2"/>
+    <sheet name="one_N" sheetId="4" r:id="rId2"/>
+    <sheet name="two" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -1508,7 +1510,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="F1" sqref="F1:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1517,7 +1519,7 @@
     <col min="12" max="12" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1530,20 +1532,8 @@
       <c r="D1">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1">
-        <v>1</v>
-      </c>
-      <c r="H1">
-        <v>2</v>
-      </c>
-      <c r="I1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1556,20 +1546,8 @@
       <c r="D2" s="1">
         <v>89.088999999999999</v>
       </c>
-      <c r="F2" s="3">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2">
-        <v>2.9491000000000001</v>
-      </c>
-      <c r="H2" s="2">
-        <v>6.7427999999999999</v>
-      </c>
-      <c r="I2" s="2">
-        <v>10.3971</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1582,20 +1560,8 @@
       <c r="D3">
         <v>23.5258</v>
       </c>
-      <c r="F3">
-        <v>20</v>
-      </c>
-      <c r="G3" s="2">
-        <v>2.9874999999999998</v>
-      </c>
-      <c r="H3" s="2">
-        <v>6.9401999999999999</v>
-      </c>
-      <c r="I3" s="2">
-        <v>10.9154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1608,20 +1574,8 @@
       <c r="D4">
         <v>12.9458</v>
       </c>
-      <c r="F4">
-        <v>40</v>
-      </c>
-      <c r="G4" s="2">
-        <v>2.9969000000000001</v>
-      </c>
-      <c r="H4" s="2">
-        <v>6.9877000000000002</v>
-      </c>
-      <c r="I4" s="2">
-        <v>11.0383</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1634,20 +1588,8 @@
       <c r="D5">
         <v>11.0784</v>
       </c>
-      <c r="F5">
-        <v>80</v>
-      </c>
-      <c r="G5" s="2">
-        <v>2.9992000000000001</v>
-      </c>
-      <c r="H5" s="2">
-        <v>6.9995000000000003</v>
-      </c>
-      <c r="I5" s="2">
-        <v>11.0687</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1660,34 +1602,8 @@
       <c r="D6">
         <v>10.9998</v>
       </c>
-      <c r="F6">
-        <v>100</v>
-      </c>
-      <c r="G6" s="2">
-        <v>2.9994999999999998</v>
-      </c>
-      <c r="H6" s="2">
-        <v>7.0008999999999997</v>
-      </c>
-      <c r="I6" s="2">
-        <v>11.0724</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="F7">
-        <v>200</v>
-      </c>
-      <c r="G7" s="2">
-        <v>2.9998999999999998</v>
-      </c>
-      <c r="H7" s="2">
-        <v>7.0027999999999997</v>
-      </c>
-      <c r="I7" s="2">
-        <v>11.077199999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
@@ -1699,11 +1615,124 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF168B5-0B5A-484C-9B09-AE7D194F37C1}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2.9491000000000001</v>
+      </c>
+      <c r="C2" s="2">
+        <v>6.7427999999999999</v>
+      </c>
+      <c r="D2" s="2">
+        <v>10.3971</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2.9874999999999998</v>
+      </c>
+      <c r="C3" s="2">
+        <v>6.9401999999999999</v>
+      </c>
+      <c r="D3" s="2">
+        <v>10.9154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>40</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2.9969000000000001</v>
+      </c>
+      <c r="C4" s="2">
+        <v>6.9877000000000002</v>
+      </c>
+      <c r="D4" s="2">
+        <v>11.0383</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>80</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2.9992000000000001</v>
+      </c>
+      <c r="C5" s="2">
+        <v>6.9995000000000003</v>
+      </c>
+      <c r="D5" s="2">
+        <v>11.0687</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>100</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2.9994999999999998</v>
+      </c>
+      <c r="C6" s="2">
+        <v>7.0008999999999997</v>
+      </c>
+      <c r="D6" s="2">
+        <v>11.0724</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>200</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2.9998999999999998</v>
+      </c>
+      <c r="C7" s="2">
+        <v>7.0027999999999997</v>
+      </c>
+      <c r="D7" s="2">
+        <v>11.077199999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{963E3408-EB3B-4913-9121-C3079CB334AC}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>